<commit_message>
create Unit test for 2 new api reviewDetail/HrVerify and reviewDetail/HeadPmVerify
</commit_message>
<xml_diff>
--- a/aspnet-core/test/Timesheet.Application.Tests/Tables/dbo.ReviewDetails.xlsx
+++ b/aspnet-core/test/Timesheet.Application.Tests/Tables/dbo.ReviewDetails.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\ncc-erp-timesheet\aspnet-core\test\Timesheet.Application.Tests\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\timesheet\git\ncc-erp-timesheet\aspnet-core\test\Timesheet.Application.Tests\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3293DBE3-C629-4B29-AA18-ED2A39E75D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -214,17 +215,29 @@
   </si>
   <si>
     <t>Reviewed</t>
+  </si>
+  <si>
+    <t>PmReviewed</t>
+  </si>
+  <si>
+    <t>HrApproved</t>
+  </si>
+  <si>
+    <t>ReOpen</t>
+  </si>
+  <si>
+    <t>Rejected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,7 +298,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -589,23 +602,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.8984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1595,6 +1611,218 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" t="s">
+        <v>63</v>
+      </c>
+      <c r="P19" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19">
+        <v>2000000</v>
+      </c>
+      <c r="U19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" t="s">
+        <v>64</v>
+      </c>
+      <c r="P20" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20">
+        <v>2000000</v>
+      </c>
+      <c r="U20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21">
+        <v>2000000</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>12</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>52</v>
+      </c>
+      <c r="S22">
+        <v>2000000</v>
+      </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Feature/52266 +: [Review intern] improve review intern (#8)
* add migration: create table ReviewInternComments

* edit api reviewDetail/GetAllDetails and reviewDetail/PMReviewInternCapability, add new api reviewDetail/HrVerify and reviewDetail/HeadPmVerify

* Feature/52266-FE

* create Unit test for 2 new api reviewDetail/HrVerify and reviewDetail/HeadPmVerify

* rename entity, add create field for private note

* rename file

* refactor query for api reviewDetail/getAllDetail

* sua code feature/52266

* remove old data PrivatenNote when PM review again

* fix code

* fix enum

* fix enum 2

---------

Co-authored-by: Duy <quangduy04072001@gmail.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/test/Timesheet.Application.Tests/Tables/dbo.ReviewDetails.xlsx
+++ b/aspnet-core/test/Timesheet.Application.Tests/Tables/dbo.ReviewDetails.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\ncc-erp-timesheet\aspnet-core\test\Timesheet.Application.Tests\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\timesheet\git\ncc-erp-timesheet\aspnet-core\test\Timesheet.Application.Tests\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3293DBE3-C629-4B29-AA18-ED2A39E75D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -214,17 +215,29 @@
   </si>
   <si>
     <t>Reviewed</t>
+  </si>
+  <si>
+    <t>PmReviewed</t>
+  </si>
+  <si>
+    <t>HrApproved</t>
+  </si>
+  <si>
+    <t>ReOpen</t>
+  </si>
+  <si>
+    <t>Rejected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,7 +298,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -589,23 +602,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.8984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1595,6 +1611,218 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" t="s">
+        <v>63</v>
+      </c>
+      <c r="P19" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19">
+        <v>2000000</v>
+      </c>
+      <c r="U19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" t="s">
+        <v>64</v>
+      </c>
+      <c r="P20" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20">
+        <v>2000000</v>
+      </c>
+      <c r="U20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21">
+        <v>2000000</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>12</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>52</v>
+      </c>
+      <c r="S22">
+        <v>2000000</v>
+      </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>